<commit_message>
Created file to make current model, added files
</commit_message>
<xml_diff>
--- a/Juan_Work/added reactions.xlsx
+++ b/Juan_Work/added reactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="132" windowWidth="12912" windowHeight="6252"/>
+    <workbookView xWindow="240" yWindow="192" windowWidth="12912" windowHeight="6192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
   <si>
     <t>asparagine biosythesis II</t>
   </si>
@@ -159,10 +159,6 @@
     <t>Formate_c0 + H_e0  -&gt; CO2_c0 + H2_c0</t>
   </si>
   <si>
-    <t>2.3.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>aconitase</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,6 +208,78 @@
   <si>
     <t>gene ID (not associate yet)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reactions in 04/15 M_mar that aren't in original</t>
+  </si>
+  <si>
+    <t>Name in model (if diff)</t>
+  </si>
+  <si>
+    <t>In new model that aren't here:</t>
+  </si>
+  <si>
+    <t>Nitrogen fixation</t>
+  </si>
+  <si>
+    <t>PFK ADP_c0</t>
+  </si>
+  <si>
+    <t>EC 1.2.1</t>
+  </si>
+  <si>
+    <t>ADP_glucokinase</t>
+  </si>
+  <si>
+    <t>Reactions in new_model (DDEs deleted) that aren't in 4/15 M_mar</t>
+  </si>
+  <si>
+    <t>Reactions in newest (4) not in prev (3)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>2.3.3.1</t>
+  </si>
+  <si>
+    <t>Citrate Synthase</t>
+  </si>
+  <si>
+    <t>Sulfopyruvate decarboxylase</t>
+  </si>
+  <si>
+    <t>Sulfolactate dehydrogenase</t>
+  </si>
+  <si>
+    <t>2_Phosphosulfolactate_phosphohydrolase</t>
+  </si>
+  <si>
+    <t>Diaminopimelate_aminotransferase</t>
+  </si>
+  <si>
+    <t>Citramalate_synthase</t>
+  </si>
+  <si>
+    <t>Isopropylmalate_isomerase_I</t>
+  </si>
+  <si>
+    <t>Isopropylmalate_isomerase_II</t>
+  </si>
+  <si>
+    <t>Methylmalate_dehydrogenase</t>
+  </si>
+  <si>
+    <t>Acetohydroxybutanoate_synthase</t>
+  </si>
+  <si>
+    <t>Acetohydroxy_acid_isomeroreductase</t>
+  </si>
+  <si>
+    <t>Gene ass.</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -250,12 +318,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,27 +358,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,259 +687,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="93.109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1">
+      <c r="A2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1">
+      <c r="A3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1">
+      <c r="A4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1">
+      <c r="A5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1">
+      <c r="A6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1">
+      <c r="A7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1">
+      <c r="A8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1">
+      <c r="A9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1">
+      <c r="A10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="7" customFormat="1">
+      <c r="A11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="7" customFormat="1">
+      <c r="A12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1">
+      <c r="A13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="7" customFormat="1">
+      <c r="A14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="7" customFormat="1">
+      <c r="A15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="7" customFormat="1">
+      <c r="A16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1">
+      <c r="A17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1">
+      <c r="A18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1">
+      <c r="A19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1">
+      <c r="A20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1">
+      <c r="A21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1">
+      <c r="A22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
+    <row r="26" spans="1:5">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>